<commit_message>
Implemented a few Feature requests
</commit_message>
<xml_diff>
--- a/Issue Tracker.xlsx
+++ b/Issue Tracker.xlsx
@@ -13,15 +13,16 @@
   </sheets>
   <definedNames>
     <definedName name="A">Sheet1!$A:$A</definedName>
-    <definedName name="Detail">Sheet1!$C:$C</definedName>
+    <definedName name="Detail">Sheet1!$D:$D</definedName>
     <definedName name="Issue">Sheet1!$A:$A</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Multiple Client's have slight difference in Title</t>
   </si>
@@ -39,6 +40,45 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>We need sort function on ally.</t>
+  </si>
+  <si>
+    <t>In the Ally menu, there are two types of sorts: by Attack type (i.e. by melee, missile, and magic) and by power (i.e. ground, air, sea). We need the bot method to be able to sort the ally list by these categories.</t>
+  </si>
+  <si>
+    <t>Issue Type</t>
+  </si>
+  <si>
+    <t>Bugfix</t>
+  </si>
+  <si>
+    <t>Feature Request</t>
+  </si>
+  <si>
+    <t>Sort allies, but remove filters if none are found</t>
+  </si>
+  <si>
+    <t>Would like a feature that adds to the sort allies feature. If an ally is not found, we'd like to remove the TYPE filter and see choose whichever ally is available.</t>
+  </si>
+  <si>
+    <t>Need a feature that can do quest progression</t>
+  </si>
+  <si>
+    <t>Need to be able to progress through the quest scenarios.</t>
+  </si>
+  <si>
+    <t>First Unit's cost is too high, cannot deploy unit</t>
+  </si>
+  <si>
+    <t>Usually the script deploys the first unit. Some quests's max unit points is less than the cost of the first unit, so the script will attempt to deploy the first unit, but it never will be able to do that.</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Made it so that the script will pick any of the 4 units when possible instead of just the first unit</t>
   </si>
 </sst>
 </file>
@@ -86,8 +126,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -383,40 +451,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="43" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfix Fixed script from stopping at unit selection page
</commit_message>
<xml_diff>
--- a/Issue Tracker.xlsx
+++ b/Issue Tracker.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Multiple Client's have slight difference in Title</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Made it so that the script will pick any of the 4 units when possible instead of just the first unit</t>
+  </si>
+  <si>
+    <t>Bot stopped responding at unit selection page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bot just stops at the unit selection page. </t>
   </si>
 </sst>
 </file>
@@ -451,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,6 +561,20 @@
       </c>
       <c r="E6" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfix Removed dumb stuff
</commit_message>
<xml_diff>
--- a/Issue Tracker.xlsx
+++ b/Issue Tracker.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Multiple Client's have slight difference in Title</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t xml:space="preserve">Bot just stops at the unit selection page. </t>
+  </si>
+  <si>
+    <t>Script doesn't work for screen size 1102 by 677</t>
+  </si>
+  <si>
+    <t>Need to make script work for that screen size</t>
   </si>
 </sst>
 </file>
@@ -457,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,6 +581,14 @@
       </c>
       <c r="D7" s="2" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorganized library functions hierarchy
</commit_message>
<xml_diff>
--- a/Issue Tracker.xlsx
+++ b/Issue Tracker.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>Multiple Client's have slight difference in Title</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>Need to make script work for that screen size</t>
+  </si>
+  <si>
+    <t>Need to support 632 by 1030</t>
+  </si>
+  <si>
+    <t>After Deploy 1 unit, bot just sits there</t>
+  </si>
+  <si>
+    <t>Bot needs to retry failed quests</t>
+  </si>
+  <si>
+    <t>Edit the BotAllQuests.ahk</t>
   </si>
 </sst>
 </file>
@@ -463,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,8 +599,41 @@
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added frontlines event support
</commit_message>
<xml_diff>
--- a/Issue Tracker.xlsx
+++ b/Issue Tracker.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="2151104" sheetId="2" r:id="rId2"/>
+    <sheet name="20151105" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="A">Sheet1!$A:$A</definedName>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Multiple Client's have slight difference in Title</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>Edit the BotAllQuests.ahk</t>
+  </si>
+  <si>
+    <t>Deploy ally makes game stuck</t>
+  </si>
+  <si>
+    <t>When there is not enough allies, the bot clicks the next page but it gets to the last page and still tries to find the next page button, but I can't. so it gets stuck</t>
+  </si>
+  <si>
+    <t>Add script for Frontlines Event</t>
+  </si>
+  <si>
+    <t>Want to automated the frontlines event.</t>
   </si>
 </sst>
 </file>
@@ -477,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,24 +655,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="142.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added frontline support for 632 by 1030 screen size
</commit_message>
<xml_diff>
--- a/Issue Tracker.xlsx
+++ b/Issue Tracker.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>Multiple Client's have slight difference in Title</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Want to automated the frontlines event.</t>
+  </si>
+  <si>
+    <t>Add support for screen size of 632 by 1030</t>
   </si>
 </sst>
 </file>
@@ -703,10 +706,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,6 +745,14 @@
         <v>30</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>